<commit_message>
add ability to supply row to read data from
</commit_message>
<xml_diff>
--- a/data/plain.xlsx
+++ b/data/plain.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dshvedchenko/projects/chnu/ml_2023S/lab4/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2B1C653-31FE-B048-9D68-B26D19701971}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C7C2F20-978B-6444-8482-A3CB872F6202}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3440" yWindow="1500" windowWidth="28040" windowHeight="17440" xr2:uid="{E45D73C9-A17B-EF4B-AB7F-5F54C60889DF}"/>
   </bookViews>
@@ -241,7 +241,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -274,7 +274,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -592,7 +592,7 @@
   <dimension ref="A2:BO4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="AC3" sqref="AC3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -803,6 +803,98 @@
         <v>65</v>
       </c>
     </row>
+    <row r="3" spans="1:67" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>6</v>
+      </c>
+      <c r="E3">
+        <v>7</v>
+      </c>
+      <c r="F3">
+        <v>3</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3">
+        <v>4</v>
+      </c>
+      <c r="I3">
+        <v>5</v>
+      </c>
+      <c r="J3">
+        <v>6</v>
+      </c>
+      <c r="K3">
+        <v>23</v>
+      </c>
+      <c r="L3">
+        <v>2</v>
+      </c>
+      <c r="M3">
+        <v>45</v>
+      </c>
+      <c r="N3">
+        <v>7</v>
+      </c>
+      <c r="O3">
+        <v>8</v>
+      </c>
+      <c r="P3">
+        <v>4</v>
+      </c>
+      <c r="Q3">
+        <v>32</v>
+      </c>
+      <c r="R3">
+        <v>5</v>
+      </c>
+      <c r="S3">
+        <v>6</v>
+      </c>
+      <c r="T3">
+        <v>4</v>
+      </c>
+      <c r="U3">
+        <v>32</v>
+      </c>
+      <c r="V3">
+        <v>5</v>
+      </c>
+      <c r="W3">
+        <v>2</v>
+      </c>
+      <c r="X3">
+        <v>54</v>
+      </c>
+      <c r="Y3">
+        <v>2</v>
+      </c>
+      <c r="Z3">
+        <v>3</v>
+      </c>
+      <c r="AA3">
+        <v>2</v>
+      </c>
+      <c r="AB3">
+        <v>7</v>
+      </c>
+      <c r="AC3">
+        <v>3</v>
+      </c>
+      <c r="AD3">
+        <v>2</v>
+      </c>
+    </row>
     <row r="4" spans="1:67" x14ac:dyDescent="0.2">
       <c r="B4" s="1"/>
     </row>

</xml_diff>